<commit_message>
added first changes after correcting python
added xlrd python egg for use in diff
</commit_message>
<xml_diff>
--- a/TestSpreadSheet.xlsx
+++ b/TestSpreadSheet.xlsx
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -406,6 +406,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
testing different python parser
</commit_message>
<xml_diff>
--- a/TestSpreadSheet.xlsx
+++ b/TestSpreadSheet.xlsx
@@ -20,9 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>formula in A3</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>World</t>
+  </si>
+  <si>
+    <t>!</t>
   </si>
 </sst>
 </file>
@@ -391,14 +400,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -413,7 +438,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -439,7 +464,11 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>A4*7</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing new xlsx parser w/ formulae
</commit_message>
<xml_diff>
--- a/TestSpreadSheet.xlsx
+++ b/TestSpreadSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15220" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -402,7 +402,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -437,7 +437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -464,11 +464,11 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <f>A4*7</f>
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working xlsx parser with formulae
</commit_message>
<xml_diff>
--- a/TestSpreadSheet.xlsx
+++ b/TestSpreadSheet.xlsx
@@ -438,7 +438,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -464,10 +464,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4">
-        <f>A4*7</f>
+        <f>A4*4</f>
         <v>28</v>
       </c>
     </row>

</xml_diff>